<commit_message>
updating lawn sign list
updating lawn sign list
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign List.xlsx
+++ b/campaign/Lawn Sign List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
   <si>
     <t>Street Number</t>
   </si>
@@ -33,9 +33,6 @@
     <t>KUMAR</t>
   </si>
   <si>
-    <t>LEE</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -193,6 +190,60 @@
   </si>
   <si>
     <t>KULAR</t>
+  </si>
+  <si>
+    <t>32 X 48</t>
+  </si>
+  <si>
+    <t>18 X 24</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Catalpa Rd</t>
+  </si>
+  <si>
+    <t>MAHASE</t>
+  </si>
+  <si>
+    <t>Brandon Gate Dr</t>
+  </si>
+  <si>
+    <t>KeMRAJH / SULAYMAN</t>
+  </si>
+  <si>
+    <t>APPLETON</t>
+  </si>
+  <si>
+    <t>Keenan Crescent</t>
+  </si>
+  <si>
+    <t>MANGAT</t>
+  </si>
+  <si>
+    <t>GANESH</t>
+  </si>
+  <si>
+    <t>DHARMAIT</t>
+  </si>
+  <si>
+    <t>ALI</t>
+  </si>
+  <si>
+    <t>HANDA</t>
+  </si>
+  <si>
+    <t>COELHO</t>
+  </si>
+  <si>
+    <t>Darla Dr</t>
+  </si>
+  <si>
+    <t>Middlebrook Dr</t>
+  </si>
+  <si>
+    <t>MiddleShire Dr</t>
   </si>
 </sst>
 </file>
@@ -216,7 +267,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -254,11 +305,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -269,6 +331,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -644,7 +711,7 @@
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,8 +721,14 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>238</v>
       </c>
@@ -665,8 +738,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>286</v>
       </c>
@@ -676,10 +752,13 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -687,10 +766,13 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>293</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -698,10 +780,13 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -709,10 +794,13 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>226</v>
+        <v>281</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -720,274 +808,343 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
-        <v>268</v>
+        <v>5065</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <v>5065</v>
+        <v>778</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>782</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2">
-        <v>778</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <v>782</v>
+        <v>648</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>655</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2">
-        <v>648</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <v>655</v>
+        <v>633</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>637</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2">
-        <v>633</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>645</v>
+        <v>616</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>632</v>
+      </c>
+      <c r="B18" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2">
-        <v>616</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
-        <v>632</v>
+        <v>5186</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2">
-        <v>5186</v>
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
       <c r="C21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
         <v>41</v>
       </c>
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3">
+        <v>3295</v>
+      </c>
       <c r="B26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C26" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="3">
-        <v>3295</v>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2">
+        <v>3296</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="E27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
-        <v>3296</v>
+        <v>7304</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="2">
-        <v>7304</v>
+        <v>3132</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2">
+        <v>3144</v>
+      </c>
+      <c r="B30" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="2">
-        <v>3132</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
       </c>
       <c r="C30" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="2">
-        <v>3144</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:5">
       <c r="A32" s="2">
-        <v>138</v>
+        <v>220</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -995,10 +1152,13 @@
       <c r="C32" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -1006,75 +1166,223 @@
       <c r="C33" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
-        <v>226</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
-        <v>266</v>
+        <v>285</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3">
+        <v>621</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2">
-        <v>285</v>
-      </c>
-      <c r="B36" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="3">
-        <v>621</v>
-      </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4">
+        <v>3695</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4">
-        <v>3695</v>
-      </c>
-      <c r="B38" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>3710</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39">
-        <v>3710</v>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="7">
+        <v>7423</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="7">
+        <v>3755</v>
+      </c>
+      <c r="B40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7">
+        <v>3785</v>
+      </c>
+      <c r="B41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="7">
+        <v>3819</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="7">
+        <v>3821</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="7">
+        <v>3826</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="7">
+        <v>7613</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7">
+        <v>3754</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="7">
+        <v>7495</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="7">
+        <v>7497</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
lawn sign list separated by region
lawn sign list separated by region
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign List.xlsx
+++ b/campaign/Lawn Sign List.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$26</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
   <si>
     <t>Street Number</t>
   </si>
@@ -244,14 +247,28 @@
   </si>
   <si>
     <t>MiddleShire Dr</t>
+  </si>
+  <si>
+    <t>Malton Lawn Sign Locations</t>
+  </si>
+  <si>
+    <t>Britannia Woods Lawn Sign Locations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -267,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -316,11 +333,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -336,6 +362,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -729,28 +758,23 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="2">
-        <v>238</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
+      <c r="A2" s="9"/>
+      <c r="B2" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
-        <v>286</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>60</v>
@@ -758,13 +782,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -772,13 +796,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2">
-        <v>238</v>
+        <v>293</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -786,13 +810,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>60</v>
@@ -800,13 +824,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2">
-        <v>281</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>60</v>
@@ -814,55 +838,55 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2">
-        <v>5065</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <v>778</v>
+        <v>5065</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>60</v>
@@ -870,55 +894,55 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <v>648</v>
+        <v>782</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <v>633</v>
+        <v>655</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>60</v>
@@ -926,27 +950,27 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <v>645</v>
+        <v>637</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <v>616</v>
+        <v>645</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
@@ -954,13 +978,13 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2">
-        <v>632</v>
+        <v>616</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" t="s">
         <v>60</v>
@@ -968,315 +992,304 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2">
+        <v>632</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
         <v>5186</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>32</v>
+      <c r="A21" s="2">
+        <v>138</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>34</v>
+      <c r="A22" s="2">
+        <v>220</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
-      </c>
-      <c r="E22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>36</v>
+      <c r="A23" s="2">
+        <v>226</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>38</v>
+      <c r="A24" s="2">
+        <v>266</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>40</v>
+      <c r="A25" s="2">
+        <v>285</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3">
+        <v>621</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3">
         <v>3295</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B35" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="2">
+      <c r="E35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2">
         <v>3296</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B36" t="s">
         <v>42</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C36" t="s">
         <v>44</v>
       </c>
-      <c r="E27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="2">
+      <c r="E36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2">
         <v>7304</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B37" t="s">
         <v>45</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C37" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="2">
+      <c r="D37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2">
         <v>3132</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B38" t="s">
         <v>47</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C38" t="s">
         <v>48</v>
       </c>
-      <c r="D29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="2">
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2">
         <v>3144</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B39" t="s">
         <v>47</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C39" t="s">
         <v>49</v>
       </c>
-      <c r="D30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="2">
-        <v>138</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="2">
-        <v>220</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2">
-        <v>226</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>52</v>
-      </c>
-      <c r="D33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2">
-        <v>266</v>
-      </c>
-      <c r="B34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" t="s">
-        <v>53</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2">
-        <v>285</v>
-      </c>
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3">
-        <v>621</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="4">
+      <c r="D39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4">
         <v>3695</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38">
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
         <v>3710</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="7">
-        <v>7423</v>
-      </c>
-      <c r="B39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="7">
-        <v>3755</v>
-      </c>
-      <c r="B40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="7">
-        <v>3785</v>
-      </c>
-      <c r="B41" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>65</v>
       </c>
       <c r="D41" t="s">
         <v>60</v>
@@ -1284,13 +1297,13 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="7">
-        <v>3819</v>
+        <v>7423</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E42" t="s">
         <v>60</v>
@@ -1298,55 +1311,55 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="7">
-        <v>3821</v>
+        <v>3755</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="7">
-        <v>3826</v>
+        <v>3785</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7">
-        <v>7613</v>
+        <v>3819</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="7">
-        <v>3754</v>
+        <v>3821</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
         <v>60</v>
@@ -1354,13 +1367,13 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="7">
-        <v>7495</v>
+        <v>3826</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" t="s">
-        <v>22</v>
+        <v>66</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>69</v>
       </c>
       <c r="E47" t="s">
         <v>60</v>
@@ -1368,19 +1381,68 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7">
+        <v>7613</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="7">
+        <v>3754</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="7">
+        <v>7495</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7">
         <v>7497</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B51" t="s">
         <v>75</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C51" t="s">
         <v>72</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E51" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E26">
+    <filterColumn colId="4"/>
+  </autoFilter>
+  <mergeCells count="2">
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding filter to lawn sign list
adding filter to lawn sign list
</commit_message>
<xml_diff>
--- a/campaign/Lawn Sign List.xlsx
+++ b/campaign/Lawn Sign List.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Britannia Woods" sheetId="1" r:id="rId1"/>
+    <sheet name="Malton" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Britannia Woods'!$A$1:$E$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Malton!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
   <si>
     <t>Street Number</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>MiddleShire Dr</t>
-  </si>
-  <si>
-    <t>Malton Lawn Sign Locations</t>
   </si>
   <si>
     <t>Britannia Woods Lawn Sign Locations</t>
@@ -258,8 +255,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,7 +281,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -304,21 +301,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -346,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -355,16 +337,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,6 +419,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -450,7 +435,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="78DC78"/>
+        <a:sysClr val="window" lastClr="7DE17D"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -517,6 +502,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -551,6 +537,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -726,21 +713,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,23 +738,23 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="9"/>
-      <c r="B2" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>238</v>
       </c>
@@ -780,7 +768,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>286</v>
       </c>
@@ -794,7 +782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>293</v>
       </c>
@@ -808,7 +796,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>238</v>
       </c>
@@ -822,7 +810,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>226</v>
       </c>
@@ -836,7 +824,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>281</v>
       </c>
@@ -850,7 +838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>268</v>
       </c>
@@ -864,7 +852,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>5065</v>
       </c>
@@ -878,7 +866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>778</v>
       </c>
@@ -892,7 +880,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>782</v>
       </c>
@@ -906,7 +894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>648</v>
       </c>
@@ -920,7 +908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>655</v>
       </c>
@@ -934,7 +922,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>633</v>
       </c>
@@ -948,7 +936,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>637</v>
       </c>
@@ -962,7 +950,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>645</v>
       </c>
@@ -976,7 +964,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>616</v>
       </c>
@@ -990,7 +978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>632</v>
       </c>
@@ -1004,7 +992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>5186</v>
       </c>
@@ -1018,7 +1006,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>138</v>
       </c>
@@ -1032,7 +1020,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>220</v>
       </c>
@@ -1046,7 +1034,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>226</v>
       </c>
@@ -1060,7 +1048,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>266</v>
       </c>
@@ -1074,7 +1062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>285</v>
       </c>
@@ -1088,7 +1076,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>621</v>
       </c>
@@ -1102,345 +1090,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="3"/>
-      <c r="B28" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="10"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="3">
-        <v>3295</v>
-      </c>
-      <c r="B35" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2">
-        <v>3296</v>
-      </c>
-      <c r="B36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2">
-        <v>7304</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2">
-        <v>3132</v>
-      </c>
-      <c r="B38" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2">
-        <v>3144</v>
-      </c>
-      <c r="B39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="4">
-        <v>3695</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41">
-        <v>3710</v>
-      </c>
-      <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="7">
-        <v>7423</v>
-      </c>
-      <c r="B42" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="7">
-        <v>3755</v>
-      </c>
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="7">
-        <v>3785</v>
-      </c>
-      <c r="B44" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" t="s">
-        <v>65</v>
-      </c>
-      <c r="D44" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="7">
-        <v>3819</v>
-      </c>
-      <c r="B45" t="s">
-        <v>66</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="7">
-        <v>3821</v>
-      </c>
-      <c r="B46" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="7">
-        <v>3826</v>
-      </c>
-      <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="7">
-        <v>7613</v>
-      </c>
-      <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" t="s">
-        <v>70</v>
-      </c>
-      <c r="D48" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="7">
-        <v>3754</v>
-      </c>
-      <c r="B49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C49" t="s">
-        <v>71</v>
-      </c>
-      <c r="E49" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="7">
-        <v>7495</v>
-      </c>
-      <c r="B50" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="7">
-        <v>7497</v>
-      </c>
-      <c r="B51" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" t="s">
-        <v>60</v>
-      </c>
-    </row>
   </sheetData>
   <autoFilter ref="A1:E26">
-    <filterColumn colId="4"/>
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
   </autoFilter>
-  <mergeCells count="2">
-    <mergeCell ref="B28:C28"/>
+  <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1449,25 +1111,370 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>3295</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>3296</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7304</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>3132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>3695</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3710</v>
+      </c>
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>7423</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>3755</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>3785</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>3819</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>3821</v>
+      </c>
+      <c r="B19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>3826</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>7613</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>3754</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>7495</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>7497</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E24">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>